<commit_message>
update to latest milestones
</commit_message>
<xml_diff>
--- a/Reports_Documentation/Report Spreadsheet.xlsx
+++ b/Reports_Documentation/Report Spreadsheet.xlsx
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t>Administrator Reports</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>add checks if time</t>
+  </si>
+  <si>
+    <t>order by job fill status so that filled jobs get sent to the bottom, removed redundant information user can see by clicking on job details</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -944,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,8 +990,11 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>50</v>
+      <c r="B4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added one bug into the spreadsheet
</commit_message>
<xml_diff>
--- a/Reports_Documentation/Report Spreadsheet.xlsx
+++ b/Reports_Documentation/Report Spreadsheet.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Reports_Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20256" windowHeight="7644"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20250" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +27,7 @@
     <author>Marcus L</author>
   </authors>
   <commentList>
-    <comment ref="A68" authorId="0" shapeId="0">
+    <comment ref="A68" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A69" authorId="0" shapeId="0">
+    <comment ref="A69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0" shapeId="0">
+    <comment ref="A70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A71" authorId="0" shapeId="0">
+    <comment ref="A71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0" shapeId="0">
+    <comment ref="A72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A73" authorId="0" shapeId="0">
+    <comment ref="A73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A74" authorId="0" shapeId="0">
+    <comment ref="A74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A75" authorId="0" shapeId="0">
+    <comment ref="A75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A76" authorId="0" shapeId="0">
+    <comment ref="A76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A77" authorId="0" shapeId="0">
+    <comment ref="A77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -471,12 +469,6 @@
     <t>add checks if time</t>
   </si>
   <si>
-    <t>order by job fill status so that filled jobs get sent to the bottom, removed redundant information user can see by clicking on job details</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>completed</t>
   </si>
   <si>
@@ -502,45 +494,66 @@
   </si>
   <si>
     <t>working</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">order by job fill status so that filled jobs get sent to the bottom, removed redundant information user can see by clicking on job details. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bug: One job in the main page was "application submitted", but it didn't show in the Manage Applications</t>
+    </r>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed, still under testing</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -548,7 +561,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -575,7 +588,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -583,7 +596,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -591,8 +604,23 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -700,14 +728,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="计算" xfId="4" builtinId="22"/>
+    <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -762,7 +818,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +853,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,28 +1030,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="64.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.625" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="43.9" customHeight="1">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1006,35 +1062,35 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="33" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="66" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>66</v>
+      <c r="B4" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="27.6" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1045,29 +1101,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="66.599999999999994" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="27">
       <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1089,7 +1145,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1097,7 +1153,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1105,7 +1161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1113,13 +1169,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1130,7 +1186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1138,7 +1194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="27">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1149,36 +1205,36 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="54">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="18.75">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="27">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1186,7 +1242,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="27">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -1194,7 +1250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="27">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -1202,7 +1258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="27">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -1210,7 +1266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="27">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1218,7 +1274,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="27">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1226,7 +1282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="27">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
@@ -1234,7 +1290,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="27">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1242,62 +1298,62 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="18.75">
       <c r="A35" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="28.5">
       <c r="A48" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="18.75">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" s="1"/>
     </row>
-    <row r="67" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="18.75">
       <c r="A67" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="15.75">
       <c r="A68" s="3">
         <v>1</v>
       </c>
@@ -1305,7 +1361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="15.75">
       <c r="A69" s="3">
         <v>2</v>
       </c>
@@ -1316,7 +1372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" s="4">
         <v>3</v>
       </c>
@@ -1324,7 +1380,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" s="4">
         <v>4</v>
       </c>
@@ -1332,7 +1388,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" s="4">
         <v>5</v>
       </c>
@@ -1340,7 +1396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" s="4">
         <v>6</v>
       </c>
@@ -1351,7 +1407,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" s="4">
         <v>7</v>
       </c>
@@ -1359,7 +1415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3">
       <c r="A75" s="4">
         <v>8</v>
       </c>
@@ -1367,7 +1423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3">
       <c r="A76" s="4">
         <v>9</v>
       </c>
@@ -1375,7 +1431,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" s="4">
         <v>10</v>
       </c>
@@ -1383,26 +1439,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="35.450000000000003" customHeight="1">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" ht="18.75">
       <c r="A81" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="27">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1474,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="27">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
@@ -1429,7 +1485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -1437,7 +1493,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="27">
       <c r="A88" s="1" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1509,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
         <v>20</v>
       </c>
@@ -1461,21 +1517,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" ht="18.75">
       <c r="A93" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="31.5">
       <c r="A94" s="6" t="s">
         <v>12</v>
       </c>
@@ -1483,27 +1539,27 @@
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="15.75">
       <c r="A95" s="6"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3">
       <c r="A99" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3">
       <c r="A103" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="27">
       <c r="A104" s="1" t="s">
         <v>17</v>
       </c>
@@ -1511,7 +1567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="67.5">
       <c r="A105" s="1" t="s">
         <v>28</v>
       </c>
@@ -1519,35 +1575,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3">
       <c r="A107" s="1"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1">
       <c r="A113" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" ht="54">
       <c r="A114" s="1" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>